<commit_message>
Added KR implementation with manual mapping and fixed bug
</commit_message>
<xml_diff>
--- a/lab4_text_search/time_results.xlsx
+++ b/lab4_text_search/time_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mwasilew\sem2\AISDI\lab4\lab4_text_search\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mkowal21\aisdi-21l\lab4_text_search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4727A985-6572-4282-A92D-403BD276F19B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0611ED-EDC7-40BB-889C-07BDD4AC9E62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>KMP</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>[min]</t>
+  </si>
+  <si>
+    <t>RK map</t>
   </si>
 </sst>
 </file>
@@ -267,31 +270,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>9.6351900100708008</c:v>
+                  <c:v>11.0252435207366</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.789641857147199</c:v>
+                  <c:v>22.217896461486799</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.1198649406433</c:v>
+                  <c:v>32.426133155822697</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38.0802035331726</c:v>
+                  <c:v>42.886498451232903</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43.286499738693202</c:v>
+                  <c:v>50.217077255249002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>52.368745803833001</c:v>
+                  <c:v>60.897600889205897</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64.327826499938894</c:v>
+                  <c:v>71.2127974033355</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70.4195108413696</c:v>
+                  <c:v>81.444462537765503</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>78.925266265869098</c:v>
+                  <c:v>91.190377473831106</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -384,31 +387,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>9.7439460754394496</c:v>
+                  <c:v>10.839520931243801</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.965904951095499</c:v>
+                  <c:v>22.586315155029201</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.153873443603501</c:v>
+                  <c:v>33.453541040420497</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39.999307394027703</c:v>
+                  <c:v>44.503835439682</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.133888244628899</c:v>
+                  <c:v>51.353311777114797</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>54.505857229232703</c:v>
+                  <c:v>62.208850860595703</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>63.866010189056396</c:v>
+                  <c:v>72.7740318775177</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>73.163623094558702</c:v>
+                  <c:v>83.334170579910193</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>81.819019556045504</c:v>
+                  <c:v>93.419229269027696</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -501,31 +504,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>33.5247673988342</c:v>
+                  <c:v>37.721246719360302</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>71.074912071227999</c:v>
+                  <c:v>79.444483041763306</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>103.137853145599</c:v>
+                  <c:v>118.18561267852699</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>137.79185295104901</c:v>
+                  <c:v>157.846711635589</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>166.67645430564801</c:v>
+                  <c:v>192.30989146232599</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>201.15985941886899</c:v>
+                  <c:v>232.47558903694099</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>244.38934087753199</c:v>
+                  <c:v>270.49874472618097</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>270.88516187667801</c:v>
+                  <c:v>309.40107917785599</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>310.813759565353</c:v>
+                  <c:v>349.02213549613901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -534,6 +537,123 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-314C-488D-9082-86B2AE8465F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RK map</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$J$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>34.028421163558903</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71.563715219497595</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>106.55306077003399</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>142.31858873367301</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>176.48787260055499</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>213.18890643119801</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>250.771466732025</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>287.14094305038401</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>321.94380402565002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-49B1-4D92-91FC-46363A04D13C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1034,31 +1154,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>9.6351900100708008</c:v>
+                  <c:v>11.0252435207366</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.789641857147199</c:v>
+                  <c:v>22.217896461486799</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.1198649406433</c:v>
+                  <c:v>32.426133155822697</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38.0802035331726</c:v>
+                  <c:v>42.886498451232903</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43.286499738693202</c:v>
+                  <c:v>50.217077255249002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>52.368745803833001</c:v>
+                  <c:v>60.897600889205897</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64.327826499938894</c:v>
+                  <c:v>71.2127974033355</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70.4195108413696</c:v>
+                  <c:v>81.444462537765503</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>78.925266265869098</c:v>
+                  <c:v>91.190377473831106</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1151,31 +1271,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>9.7439460754394496</c:v>
+                  <c:v>10.839520931243801</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.965904951095499</c:v>
+                  <c:v>22.586315155029201</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.153873443603501</c:v>
+                  <c:v>33.453541040420497</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39.999307394027703</c:v>
+                  <c:v>44.503835439682</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.133888244628899</c:v>
+                  <c:v>51.353311777114797</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>54.505857229232703</c:v>
+                  <c:v>62.208850860595703</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>63.866010189056396</c:v>
+                  <c:v>72.7740318775177</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>73.163623094558702</c:v>
+                  <c:v>83.334170579910193</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>81.819019556045504</c:v>
+                  <c:v>93.419229269027696</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1268,31 +1388,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>33.5247673988342</c:v>
+                  <c:v>37.721246719360302</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>71.074912071227999</c:v>
+                  <c:v>79.444483041763306</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>103.137853145599</c:v>
+                  <c:v>118.18561267852699</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>137.79185295104901</c:v>
+                  <c:v>157.846711635589</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>166.67645430564801</c:v>
+                  <c:v>192.30989146232599</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>201.15985941886899</c:v>
+                  <c:v>232.47558903694099</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>244.38934087753199</c:v>
+                  <c:v>270.49874472618097</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>270.88516187667801</c:v>
+                  <c:v>309.40107917785599</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>310.813759565353</c:v>
+                  <c:v>349.02213549613901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1301,6 +1421,123 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-84D8-45E6-94EC-3D3D66B7736B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RK map</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$J$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>34.028421163558903</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71.563715219497595</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>106.55306077003399</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>142.31858873367301</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>176.48787260055499</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>213.18890643119801</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>250.771466732025</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>287.14094305038401</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>321.94380402565002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3486-4DA2-9694-59419C2CC0BF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2757,16 +2994,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>130492</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>111442</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2794,15 +3031,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>59055</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1200150</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>116205</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3095,9 +3332,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -3156,31 +3393,31 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>9.6351900100708008</v>
+        <v>11.0252435207366</v>
       </c>
       <c r="C2">
-        <v>18.789641857147199</v>
+        <v>22.217896461486799</v>
       </c>
       <c r="D2">
-        <v>28.1198649406433</v>
+        <v>32.426133155822697</v>
       </c>
       <c r="E2">
-        <v>38.0802035331726</v>
+        <v>42.886498451232903</v>
       </c>
       <c r="F2">
-        <v>43.286499738693202</v>
+        <v>50.217077255249002</v>
       </c>
       <c r="G2">
-        <v>52.368745803833001</v>
+        <v>60.897600889205897</v>
       </c>
       <c r="H2">
-        <v>64.327826499938894</v>
+        <v>71.2127974033355</v>
       </c>
       <c r="I2">
-        <v>70.4195108413696</v>
+        <v>81.444462537765503</v>
       </c>
       <c r="J2">
-        <v>78.925266265869098</v>
+        <v>91.190377473831106</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -3188,31 +3425,31 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>9.7439460754394496</v>
+        <v>10.839520931243801</v>
       </c>
       <c r="C3">
-        <v>20.965904951095499</v>
+        <v>22.586315155029201</v>
       </c>
       <c r="D3">
-        <v>30.153873443603501</v>
+        <v>33.453541040420497</v>
       </c>
       <c r="E3">
-        <v>39.999307394027703</v>
+        <v>44.503835439682</v>
       </c>
       <c r="F3">
-        <v>45.133888244628899</v>
+        <v>51.353311777114797</v>
       </c>
       <c r="G3">
-        <v>54.505857229232703</v>
+        <v>62.208850860595703</v>
       </c>
       <c r="H3">
-        <v>63.866010189056396</v>
+        <v>72.7740318775177</v>
       </c>
       <c r="I3">
-        <v>73.163623094558702</v>
+        <v>83.334170579910193</v>
       </c>
       <c r="J3">
-        <v>81.819019556045504</v>
+        <v>93.419229269027696</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -3220,49 +3457,81 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>33.5247673988342</v>
+        <v>37.721246719360302</v>
       </c>
       <c r="C4">
-        <v>71.074912071227999</v>
+        <v>79.444483041763306</v>
       </c>
       <c r="D4">
-        <v>103.137853145599</v>
+        <v>118.18561267852699</v>
       </c>
       <c r="E4">
-        <v>137.79185295104901</v>
+        <v>157.846711635589</v>
       </c>
       <c r="F4">
-        <v>166.67645430564801</v>
+        <v>192.30989146232599</v>
       </c>
       <c r="G4">
-        <v>201.15985941886899</v>
+        <v>232.47558903694099</v>
       </c>
       <c r="H4">
-        <v>244.38934087753199</v>
+        <v>270.49874472618097</v>
       </c>
       <c r="I4">
-        <v>270.88516187667801</v>
+        <v>309.40107917785599</v>
       </c>
       <c r="J4">
-        <v>310.813759565353</v>
+        <v>349.02213549613901</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I5" t="s">
-        <v>4</v>
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>34.028421163558903</v>
+      </c>
+      <c r="C5">
+        <v>71.563715219497595</v>
+      </c>
+      <c r="D5">
+        <v>106.55306077003399</v>
+      </c>
+      <c r="E5">
+        <v>142.31858873367301</v>
+      </c>
+      <c r="F5">
+        <v>176.48787260055499</v>
+      </c>
+      <c r="G5">
+        <v>213.18890643119801</v>
+      </c>
+      <c r="H5">
+        <v>250.771466732025</v>
+      </c>
+      <c r="I5">
+        <v>287.14094305038401</v>
       </c>
       <c r="J5">
-        <f>SUM(B2:J4)</f>
-        <v>2362.7581412792165</v>
+        <v>321.94380402565002</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <f>SUM(B2:J5)</f>
+        <v>4288.8931667804663</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
         <v>5</v>
       </c>
-      <c r="J6">
-        <f>J5/60</f>
-        <v>39.379302354653611</v>
+      <c r="J7">
+        <f>J6/60</f>
+        <v>71.481552779674445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>